<commit_message>
Add fixed capital costs to converters
</commit_message>
<xml_diff>
--- a/excel_files/General_input_new_simple.xlsx
+++ b/excel_files/General_input_new_simple.xlsx
@@ -224,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +443,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
   <si>
     <t xml:space="preserve">Annualised capital costs</t>
   </si>
@@ -469,10 +469,16 @@
     <t xml:space="preserve">BatSize</t>
   </si>
   <si>
+    <t xml:space="preserve">Grid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Units</t>
   </si>
   <si>
     <t xml:space="preserve">kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kW</t>
   </si>
   <si>
     <t xml:space="preserve">Type</t>
@@ -497,9 +503,6 @@
   </si>
   <si>
     <t xml:space="preserve">Irradiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid</t>
   </si>
   <si>
     <t xml:space="preserve">Gas</t>
@@ -542,6 +545,9 @@
   </si>
   <si>
     <t xml:space="preserve">capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed capital cost</t>
   </si>
   <si>
     <t xml:space="preserve">capital cost</t>
@@ -617,9 +623,6 @@
   </si>
   <si>
     <t xml:space="preserve">Node</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kW</t>
   </si>
   <si>
     <t xml:space="preserve">kW/m2</t>
@@ -1200,10 +1203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1223,48 +1226,60 @@
       <c r="C1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9999</v>
@@ -1306,32 +1321,32 @@
         <v>5</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1351,7 +1366,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.14</v>
@@ -1371,7 +1386,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1406,15 +1421,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.59"/>
@@ -1427,36 +1442,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>10000</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>100</v>
@@ -1465,218 +1480,223 @@
         <v>45</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>200</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>3500</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>2900</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>1000</v>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="C4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>2900</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D6" s="4" t="n">
         <v>0.01</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.021</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.06</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G6" s="4" t="n">
         <v>0.12</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H6" s="4" t="n">
         <v>0.021</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="n">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C7" s="4" t="n">
         <v>3.2</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D7" s="4" t="n">
         <v>0.94</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E7" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F7" s="4" t="n">
         <v>0.14</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G7" s="4" t="n">
         <v>0.46</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H7" s="4" t="n">
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="n">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D8" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F8" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G8" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H8" s="4" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="n">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="n">
-        <v>50</v>
+        <v>1.73</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="n">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="n">
         <v>50</v>
       </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="n">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1712,31 +1732,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -1747,7 +1767,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1</v>
@@ -1758,7 +1778,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>20</v>
@@ -1769,7 +1789,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.99</v>
@@ -1780,7 +1800,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0.99</v>
@@ -1791,7 +1811,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0.001</v>
@@ -1802,7 +1822,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>0.3</v>
@@ -1813,7 +1833,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0.3</v>
@@ -1824,7 +1844,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0</v>
@@ -1865,73 +1885,73 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>3</v>
@@ -10958,66 +10978,67 @@
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -11050,37 +11071,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -11114,62 +11135,62 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>